<commit_message>
Question Type Prompt refined
I've been working on a prompt to classify questions into the following categories: TERM, DESCRIPTION, LOCATION, TRUE, FALSE, or UNKNOWN.
</commit_message>
<xml_diff>
--- a/SAILUP-INN/uploads/sailup_per_questions_chatgpt_output.xlsx
+++ b/SAILUP-INN/uploads/sailup_per_questions_chatgpt_output.xlsx
@@ -416,7 +416,7 @@
         <v>Topic</v>
       </c>
       <c r="E1" t="str">
-        <v>Frequency</v>
+        <v>Type</v>
       </c>
       <c r="F1" t="str">
         <v>Thumbnail</v>
@@ -452,7 +452,7 @@
         <v>Summary4</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
+    <row r="2">
       <c r="A2" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -466,7 +466,7 @@
         <v>Bitas</v>
       </c>
       <c r="E2" t="str">
-        <v>H</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -489,26 +489,20 @@
       <c r="L2" t="str">
         <v>Pieza de acero moldeada que firme en cubierta sirve para dirigir los cabos en un sentido determinado.</v>
       </c>
-      <c r="M2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Una &lt;strong&gt;bita&lt;/strong&gt; es una pieza cilíndrica fijada a la cubierta de una embarcación que se utiliza para asegurar y amarrar los cabos. Su función principal es ayudar en el manejo y control de las embarcaciones durante el atraque o el amarre.</v>
-      </c>
-      <c r="N2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Una &lt;strong&gt;bita&lt;/strong&gt; es una pieza, generalmente de hierro, firme a los muelles, utilizada para asegurar las amarras de los buques.</v>
-      </c>
-      <c r="O2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta es de "definición".
-Fase 2 · Explicación: Una &lt;strong&gt;bita&lt;/strong&gt; es un dispositivo náutico en forma de T firme en la cubierta de un barco que se utiliza para amarrar y asegurar los cabos de las embarcaciones.</v>
-      </c>
-      <c r="P2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación:
-La pregunta "¿Qué es una bita?" se clasifica como "definición", ya que solicita una descripción de qué es algo.
-Fase 2 · Explicación:
-Las &lt;strong&gt;bitas&lt;/strong&gt; son estructuras firmemente fijadas en la cubierta de un barco, generalmente hechas de acero, que se utilizan para dirigir o asegurar cabos en un sentido determinado en la embarcación.</v>
-      </c>
-    </row>
-    <row r="3" xml:space="preserve">
+      <c r="M2" t="str">
+        <v>Una embarcación está &lt;strong&gt;adrizada&lt;/strong&gt; cuando navega vertical y equilibrada, sin inclinación lateral respecto a la vertical; en otras palabras, sin escora.</v>
+      </c>
+      <c r="N2" t="str">
+        <v>Se dice que una embarcación &lt;strong&gt;está en varadero&lt;/strong&gt; cuando ha sido sacada del agua y se encuentra en tierra, en un astillero o dique, para realizar trabajos de mantenimiento, reparación o invernaje.</v>
+      </c>
+      <c r="O2" t="str">
+        <v>En náutica, la expresión &lt;strong&gt;apenas se mueve&lt;/strong&gt; indica que el barco lleva una arrancada muy pequeña o casi nula, es decir, prácticamente no avanza con respecto al agua.</v>
+      </c>
+      <c r="P2" t="str">
+        <v>Una embarcación &lt;strong&gt;navega contra el viento&lt;/strong&gt; cuando avanza en dirección al viento o lo más cercano posible a él, lo que implica mayor resistencia y necesidad de ajustar el gobierno.</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -522,7 +516,7 @@
         <v>Gaza</v>
       </c>
       <c r="E3" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -545,28 +539,20 @@
       <c r="L3" t="str">
         <v>El medio nudo alrededor de una verga.</v>
       </c>
-      <c r="M3" t="str" xml:space="preserve">
-        <v xml:space="preserve">### Fase 1 · Clasificación
-Tipo de pregunta: **definición**
-### Fase 2 · Explicación
-Una **gaza** es un lazo creado en el extremo de un cabo trenzando los cordones sobre la parte firme del mismo. Se utiliza comúnmente en la náutica para formar un bucle fijo.</v>
-      </c>
-      <c r="N3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: En náutica, una &lt;strong&gt;gaza&lt;/strong&gt; es un bucle o lazo que se forma por un extremo de un cabo, útil para engancharlo a otro objeto o cabo. La opción dada describe incorrectamente la &lt;strong&gt;gaza&lt;/strong&gt;, ya que no se refiere a la curvatura del cabo entre los extremos.</v>
-      </c>
-      <c r="O3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Una &lt;strong&gt;Gaza&lt;/strong&gt; es una especie de lazo o anillo que se forma en el extremo de un cabo, utilizando un nudo, generalmente para facilitar el enganche o aseguramiento en una estructura o con otro cabo. El nudo mencionado en la opción se refiere a cómo se forma esta gaza al pasar el chicote alrededor del firme y por el seno.</v>
-      </c>
-      <c r="P3" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación**  
-Tipo de pregunta: "definición"
-**Fase 2 · Explicación**  
-Una **Gaza** es un lazo o anillo formado en el extremo de un cabo empleado en diversos contextos náuticos para asegurar o enganchar el cabo a otro objeto. No se refiere a un medio nudo alrededor de una verga; esto más bien podría estar relacionado con un tipo de amarre o sujeción.</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+      <c r="O3" t="str">
+        <v/>
+      </c>
+      <c r="P3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -580,7 +566,7 @@
         <v>Bichero</v>
       </c>
       <c r="E4" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -603,26 +589,20 @@
       <c r="L4" t="str">
         <v>Pieza de madera o metal que sale del casco horizontalmente</v>
       </c>
-      <c r="M4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta es de "definición" porque pide una definición de "bichero".
-Fase 2 · Explicación: El &lt;strong&gt;bichero&lt;/strong&gt; es una vara larga terminada en un herraje en forma de gancho en un extremo, utilizada en el ámbito náutico para facilitar el amarre, mover las embarcaciones o recoger objetos del agua.</v>
-      </c>
-      <c r="N4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición.
-Fase 2 · Explicación: Un &lt;strong&gt;bichero&lt;/strong&gt; es una vara larga que tiene un gancho en un extremo, utilizada en la náutica para tareas como recoger objetos del agua o acercar un barco a un muelle. La opción presentada no está relacionada con el término bichero en este contexto.</v>
-      </c>
-      <c r="O4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo: "definición"
-Fase 2 · Explicación  
-El término &lt;strong&gt;bichero&lt;/strong&gt; se refiere a un instrumento náutico que consiste en un palo largo con un gancho en el extremo, utilizado para manipular cabos o recoger objetos del agua desde una embarcación. No se trata de una pieza de madera para amurar el spinnaker; esa descripción no se ajusta a su verdadera función.</v>
-      </c>
-      <c r="P4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Un &lt;strong&gt;bichero&lt;/strong&gt; es una herramienta náutica, normalmente un palo largo con un gancho al final, utilizada para enganchar o empujar objetos desde una embarcación. La opción "pieza de madera o metal que sale del casco horizontalmente" no describe a un bichero; este término se refiere más bien a los puntales o defensas utilizados para proteger el casco.</v>
-      </c>
-    </row>
-    <row r="5" xml:space="preserve">
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
+        <v/>
+      </c>
+      <c r="O4" t="str">
+        <v/>
+      </c>
+      <c r="P4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -636,7 +616,7 @@
         <v>Gaza</v>
       </c>
       <c r="E5" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -659,26 +639,20 @@
       <c r="L5" t="str">
         <v>Superficie porosa apta para la limpieza de los instrumentos de precisión.</v>
       </c>
-      <c r="M5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: función
-Fase 2 · Explicación: Una &lt;strong&gt;gaza&lt;/strong&gt; es una especie de ojo formado en el extremo de un cabo, conocido como chicote, que sirve para hacer firme el cabo o enganchar algo en él. Se utiliza comúnmente en actividades marítimas para asegurar objetos de manera eficiente.</v>
-      </c>
-      <c r="N5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación
-Tipo de pregunta: genérico
-Fase 2 · Explicación
-&lt;strong&gt;Gaza&lt;/strong&gt; en náutica se refiere a un lazo o anillo ejecutado al final de un cabo utilizando varios tipos de nudos, como el nudo de gaza, para facilitar la conexión con otros cabos o con diferentes elementos en una embarcación. No está relacionada con el material de la funda del ancla.</v>
-      </c>
-      <c r="O5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: localización.
-Fase 2 · Explicación: En náutica, una &lt;strong&gt;gaza&lt;/strong&gt; es un bucle o anillo hecho al final de una cuerda o cabo. No es una "ventana situada a la derecha del buque", por lo que la definición correcta está relacionada con su uso en el manejo de cabos a bordo.</v>
-      </c>
-      <c r="P5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta es de tipo "función" porque se enfoca en el propósito o uso de la "Gaza".
-Fase 2 · Explicación: En el contexto náutico, una &lt;strong&gt;Gaza&lt;/strong&gt; es un anillo o lazo hecho en el extremo de un cabo para facilitar su empleo en distintas maniobras. La opción presentada es incorrecta ya que la gaza no se relaciona con la limpieza de instrumentos de precisión.</v>
-      </c>
-    </row>
-    <row r="6" xml:space="preserve">
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <v/>
+      </c>
+      <c r="O5" t="str">
+        <v/>
+      </c>
+      <c r="P5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -692,7 +666,7 @@
         <v>Muertos</v>
       </c>
       <c r="E6" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -715,28 +689,20 @@
       <c r="L6" t="str">
         <v>Coz</v>
       </c>
-      <c r="M6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Un &lt;strong&gt;muerto&lt;/strong&gt; es un bloque pesado colocado en el fondo de un cuerpo de agua al que se acopla una boya o baliza mediante un cable o cadena, proporcionando así un punto fijo de amarre o señalización. La opción "orinque", sin embargo, es incorrecta; ya que el término se refiere a una cuerda delgada usada para marcar la ubicación de un ancla fondeada, no al cable o cadena que sujeta una boya al muerto.</v>
-      </c>
-      <c r="N6" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación**: definición
-**Fase 2 · Explicación**: En el ámbito náutico, un &lt;strong&gt;muerto&lt;/strong&gt; es un lastre sumergido que se utiliza para asegurar una boya o baliza en una posición fija en el agua. El término "caña" no es correcto para denominar el cable o cadena que conecta una boya al muerto; generalmente se le llama "cabo" o "cadena de fondeo".</v>
-      </c>
-      <c r="O6" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:**  
-La pregunta dada es de tipo "definición" ya que se está preguntando qué es el cable o cadena que sujeta la boya o baliza al muerto.
-**Fase 2 · Explicación:**  
-Un **Muerto** es un lastre fijo en el fondo del mar que se utiliza para anclar boyas o balizas. El cable o cadena utilizado para sujetar la boya al muerto se llama "orinque", no "uña".</v>
-      </c>
-      <c r="P6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-La pregunta es de tipo "definición" porque pide qué es un término específico dentro del contexto.
-Fase 2 · Explicación  
-En el contexto náutico, el término &lt;strong&gt;Muertos&lt;/strong&gt; se refiere a una estructura sumergida y pesada utilizada para anclar bojones, boyas o balizas mediante cadenas o cables. El término "Coz" no corresponde a un concepto náutico relacionado con esta función; el término correcto para el cable o cadena que sujeta la boya al muerto es "orinque" o "cadena de fondeo".</v>
-      </c>
-    </row>
-    <row r="7" xml:space="preserve">
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <v/>
+      </c>
+      <c r="O6" t="str">
+        <v/>
+      </c>
+      <c r="P6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -750,7 +716,7 @@
         <v>Bichero</v>
       </c>
       <c r="E7" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -773,28 +739,20 @@
       <c r="L7" t="str">
         <v>Es el cabo que une un muerto con su boya en la superficie.</v>
       </c>
-      <c r="M7" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:** definición
-**Fase 2 · Explicación:** Un &lt;strong&gt;bichero&lt;/strong&gt; es una herramienta náutica que consiste en una pértiga con un gancho y una punta en su extremo, utilizada para manejar cabos, recoger objetos del agua o acercarse a muelles y otras embarcaciones.</v>
-      </c>
-      <c r="N7" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:**
-La pregunta es de tipo "definición" porque pide qué es un bichero.
-**Fase 2 · Explicación:**
-Un &lt;strong&gt;bichero&lt;/strong&gt; es una herramienta náutica que consiste en un palo largo con un gancho en un extremo, utilizado para maniobrar embarcaciones o recoger objetos flotantes en el agua. La opción presentada es incorrecta; el elemento cilíndrico relleno de corcho o aire comprimido no describe a un bichero.</v>
-      </c>
-      <c r="O7" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Un &lt;strong&gt;bichero&lt;/strong&gt; es una herramienta náutica que consiste en un palo largo con un gancho en un extremo, utilizado para recoger objetos del agua o ayudar en el atraque de embarcaciones. La opción mencionada se refiere a una bita, que es un poste cilíndrico en un muelle para amarrar barcos.</v>
-      </c>
-      <c r="P7" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación**  
-Tipo de pregunta: "verdadero_falso"
-**Fase 2 · Explicación**  
-Un &lt;strong&gt;bichero&lt;/strong&gt; no es el cabo que une un muerto con su boya en la superficie. En realidad, un &lt;strong&gt;bichero&lt;/strong&gt; es una herramienta náutica utilizada para agarrar o empujar objetos desde una embarcación mediante un mango largo con un gancho en el extremo.</v>
-      </c>
-    </row>
-    <row r="8" xml:space="preserve">
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <v/>
+      </c>
+      <c r="P7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -808,7 +766,7 @@
         <v>Gaza</v>
       </c>
       <c r="E8" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -831,30 +789,20 @@
       <c r="L8" t="str">
         <v>El doble llano.</v>
       </c>
-      <c r="M8" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación**  
-Tipo de pregunta: función
-**Fase 2 · Explicación**  
-El &lt;strong&gt;as de guía&lt;/strong&gt; es un nudo marinero que se utiliza para crear un lazo fijo en el extremo de una cuerda, sirviendo como una alternativa versátil a la &lt;strong&gt;Gaza&lt;/strong&gt;, que es un ojo hecho en un cabo.</v>
-      </c>
-      <c r="N8" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación:  
-La pregunta es de tipo "genérico" porque se refiere a una sustitución en un contexto específico, pero no encaja claramente en las otras categorías.
-Fase 2 · Explicación:  
-El &lt;strong&gt;ballestrinque&lt;/strong&gt; es un nudo utilizado principalmente para asegurar un cabo a un objeto, como una estaca o una barra, pero no es apropiado para sustituir la &lt;strong&gt;gaza&lt;/strong&gt;, que es un nudo o una modalidad de cabo que forma un bucle fijo utilizado para amarrar o asegurar elementos. Para sustituir una gaza se podría considerar un nudo de as de guía.</v>
-      </c>
-      <c r="O8" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: genérico.
-Fase 2 · Explicación: El &lt;strong&gt;nudo llano&lt;/strong&gt; es un tipo de nudo que se utiliza principalmente para unir dos cabos de igual grosor, pero no es adecuado para formar una &lt;strong&gt;gaza&lt;/strong&gt;. La función de una gaza es hacer un bucle o lazo al final de un cabo, y se logran con otros nudos específicos como el nudo de as de guía.</v>
-      </c>
-      <c r="P8" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación
-La pregunta es de tipo "verdadero_falso" porque presenta solo dos opciones (correcto o incorrecto).
-Fase 2 · Explicación
-El &lt;strong&gt;doble llano&lt;/strong&gt;, conocido también como nudo de rizo, es un nudo de unión utilizado comúnmente para unir dos cabos de igual grosor, pero no es un sustituto directo de la &lt;strong&gt;gaza&lt;/strong&gt;, la cual es un lazo o anillo en el extremo de un cabo.</v>
-      </c>
-    </row>
-    <row r="9" xml:space="preserve">
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v/>
+      </c>
+      <c r="O8" t="str">
+        <v/>
+      </c>
+      <c r="P8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -868,7 +816,7 @@
         <v>Noray</v>
       </c>
       <c r="E9" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -891,28 +839,20 @@
       <c r="L9" t="str">
         <v>Uno a proa y otro a popa de la embarcación.</v>
       </c>
-      <c r="M9" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta corresponde al tipo "localización" ya que indaga sobre dónde se encuentran los **norays**.
-Fase 2 · Explicación: Los **norays** están situados en el muelle y se utilizan para amarrar las embarcaciones.</v>
-      </c>
-      <c r="N9" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:**  
-Tipo de pregunta: "localización"
-**Fase 2 · Explicación:**  
-Un &lt;strong&gt;noray&lt;/strong&gt; es un elemento náutico que se encuentra habitualmente en los muelles para amarrar embarcaciones. No se sitúa en el costado de estribor de cubierta, ya que su ubicación corresponde a tierra firme.</v>
-      </c>
-      <c r="O9" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta es de tipo "localización" ya que está preguntando dónde se encuentran.  
-Fase 2 · Explicación: Los &lt;strong&gt;norays&lt;/strong&gt; son elementos utilizados principalmente para amarrar embarcaciones. Su ubicación habitual es en los muelles o en la cubierta de una embarcación, no en los costados de cubierta.</v>
-      </c>
-      <c r="P9" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación**  
-Tipo de pregunta: "localización"
-**Fase 2 · Explicación**  
-Un &lt;strong&gt;noray&lt;/strong&gt; es un elemento utilizado para amarrar las embarcaciones en un muelle o puerto, y no se sitúa en proa o popa de la embarcación, sino en tierra, generalmente en la estructura del muelle.</v>
-      </c>
-    </row>
-    <row r="10" xml:space="preserve">
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <v/>
+      </c>
+      <c r="O9" t="str">
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -926,7 +866,7 @@
         <v>Muertos</v>
       </c>
       <c r="E10" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -949,26 +889,20 @@
       <c r="L10" t="str">
         <v>Es un bloque pesado colgado de un flotador que lo sostiene a determinada profundidad.</v>
       </c>
-      <c r="M10" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta es de "definición" porque pide qué es un "muerto".
-Fase 2 · Explicación: Un &lt;strong&gt;muerto&lt;/strong&gt; en el contexto náutico es un bloque de hormigón u otro material pesado situado en el fondo marino, al cual se amarra el extremo de un cabo para asegurar boyas, balizas, o embarcaciones.</v>
-      </c>
-      <c r="N10" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta es de tipo "definición", ya que está solicitando que se explique qué es un "muerto" basado en la opción dada.
-Fase 2 · Explicación: En el contexto náutico, un &lt;strong&gt;muerto&lt;/strong&gt; se refiere a un cuerpo fijo en el fondo del mar que se utiliza como anclaje para asegurar embarcaciones, boyas u otros elementos flotantes. La opción presentada es incorrecta, ya que "&lt;strong&gt;cabo&lt;/strong&gt; que no trabaja" no es una definición adecuada para "muerto".</v>
-      </c>
-      <c r="O10" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación**
-Tipo de pregunta: "definición"
-**Fase 2 · Explicación**
-El término **muertos** en náutica se refiere a anclas o bloques fijos bajo el agua a los que se amarran las embarcaciones, no el extremo del cabo que queda colgando del noray. El uso indicado en la opción no corresponde correctamente a los términos marítimos comunes.</v>
-      </c>
-      <c r="P10" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:** definición
-**Fase 2 · Explicación:** Un &lt;strong&gt;muerto&lt;/strong&gt; es un ancla pesada que se coloca en el fondo del agua para mantener una posición fija de embarcaciones o estructuras flotantes, como boyas o plataformas. Normalmente se utiliza cuando no es práctico o posible utilizar anclajes convencionales.</v>
-      </c>
-    </row>
-    <row r="11" xml:space="preserve">
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <v/>
+      </c>
+      <c r="O10" t="str">
+        <v/>
+      </c>
+      <c r="P10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -982,7 +916,7 @@
         <v>Boyas</v>
       </c>
       <c r="E11" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1005,28 +939,20 @@
       <c r="L11" t="str">
         <v>Norays.</v>
       </c>
-      <c r="M11" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: "definición"
-Fase 2 · Explicación  
-Los &lt;strong&gt;Muertos&lt;/strong&gt; son bloques de hormigón firmes situados en el fondo acuático a los cuales se sujetan boyas y que permiten amarrar embarcaciones al atracar de punta. Este tipo de anclaje asegura que la boya permanezca en su posición, proporcionando un punto de amarre fijo y seguro.</v>
-      </c>
-      <c r="N11" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación:  
-- Tipo de pregunta: **definición**
-Fase 2 · Explicación:  
-Una &lt;strong&gt;boa&lt;/strong&gt; es un dispositivo flotante que se utiliza principalmente para indicar una ubicación específica en el agua o para amarrar embarcaciones de manera segura. Las bozas, en cambio, son cabos cortos y fuertes que se utilizan para sujetar un barco a un muelle o para unirlo a una boya.</v>
-      </c>
-      <c r="O11" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta es de tipo "definición", ya que pide qué es algo.
-Fase 2 · Explicación: Los &lt;strong&gt;bolardos&lt;/strong&gt; son postes cortos y robustos que se utilizan en puertos, muelles o embarcaciones para asegurar amarras de barcos y no corresponden a las estructuras de hormigón mencionadas en la pregunta original, las cuales se conocen como "muertos" o "anclas" cuando se habla de boyas.</v>
-      </c>
-      <c r="P11" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta es de "definición" porque está solicitando información sobre qué son "Norays".
-Fase 2 · Explicación: Los &lt;strong&gt;norays&lt;/strong&gt; son estructuras firmemente ancladas en los muelles o en el suelo, utilizadas para sujetar amarras y asegurar las embarcaciones en puertos o muelles, no son bloques en el fondo del mar para sujetar boyas. En el contexto solicitado, la palabra correcta sería "muertos", que son los bloques de hormigón que están en el fondo del agua para asegurar boyas u otros sistemas de amarre.</v>
-      </c>
-    </row>
-    <row r="12" xml:space="preserve">
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <v/>
+      </c>
+      <c r="O11" t="str">
+        <v/>
+      </c>
+      <c r="P11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1040,7 +966,7 @@
         <v>Cornamusas</v>
       </c>
       <c r="E12" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1063,28 +989,20 @@
       <c r="L12" t="str">
         <v>Decoraciones rústicas realizadas en determinados buques.</v>
       </c>
-      <c r="M12" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: "definición"
-Fase 2 · Explicación  
-&lt;strong&gt;Cornamusas&lt;/strong&gt; son elementos en forma de T hechos de madera o metal, fijados en diversas partes de un barco, que se utilizan para asegurar cabos o drizas.</v>
-      </c>
-      <c r="N12" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Las &lt;strong&gt;cornamusas&lt;/strong&gt;, en el contexto náutico, son piezas utilizadas en embarcaciones, principalmente de metal o madera, donde se amarran cabos o cuerdas. Su función principal es asegurar las amarras del barco, manteniéndolo en posición.</v>
-      </c>
-      <c r="O12" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Las &lt;strong&gt;cornamusas&lt;/strong&gt; son piezas en forma de T, generalmente hechas de metal o plástico, utilizadas en embarcaciones para asegurar cabos o cuerdas. Son un elemento esencial para amarrar o sujetar una embarcación en el muelle o para manejar las velas.</v>
-      </c>
-      <c r="P12" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: "definición"
-Fase 2 · Explicación  
-&lt;strong&gt;Cornamusas&lt;/strong&gt; son dispositivos en las embarcaciones utilizados para amarrar cabos. No son decoraciones, sino elementos esenciales para asegurar el barco al muelle o para otras maniobras de amarre.</v>
-      </c>
-    </row>
-    <row r="13" xml:space="preserve">
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <v/>
+      </c>
+      <c r="O12" t="str">
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1098,7 +1016,7 @@
         <v>Firme</v>
       </c>
       <c r="E13" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1121,28 +1039,20 @@
       <c r="L13" t="str">
         <v>Dejar</v>
       </c>
-      <c r="M13" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:** definición
-**Fase 2 · Explicación:** &lt;strong&gt;Firme&lt;/strong&gt; en náutica se refiere a la dirección estable y constante de un cabo o aparejo que asegura una carga o estructura. No se debe confundir con &lt;strong&gt;Largar&lt;/strong&gt;, que es la acción de soltar completamente uno o varios cabos de donde estaban firmes.</v>
-      </c>
-      <c r="N13" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta corresponde al tipo "definición", ya que busca entender qué significa la acción mencionada.
-Fase 2 · Explicación: En náutica, la acción de &lt;strong&gt;arriar&lt;/strong&gt; se refiere a bajar o soltar una vela, bandera o cualquier aparejo desde su posición tensa o elevada. Sin embargo, para la definición específica mencionada, relacionada con soltar totalmente un cabo, el término más adecuado sería "amollar" o "largar".</v>
-      </c>
-      <c r="O13" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: definición
-Fase 2 · Explicación  
-En náutica, &lt;strong&gt;lascar&lt;/strong&gt; se refiere a la acción de aflojar o soltar un cabo, generalmente desde un winche o bitas, permitiendo que se deslice para regular la tensión o posición del mismo. Esta acción es importante para ajustar las velas o evitar tensiones excesivas en el aparejo.</v>
-      </c>
-      <c r="P13" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: "definición"
-Fase 2 · Explicación  
-El término &lt;strong&gt;Firme&lt;/strong&gt; en náutica se refiere al cabo o cuerda que está bien sujeto o asegurado en su lugar, contrario al concepto de "soltar" un cabo. En este contexto, "Dejar" no es una terminología náutica específica para determinar la acción de soltar un cabo de su firmeza, ya que el término correcto sería "amollar" o "largarse".</v>
-      </c>
-    </row>
-    <row r="14" xml:space="preserve">
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v/>
+      </c>
+      <c r="O13" t="str">
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1156,7 +1066,7 @@
         <v>Defensas</v>
       </c>
       <c r="E14" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1179,26 +1089,20 @@
       <c r="L14" t="str">
         <v>Sobre los portillos para aislarlos del agua de lluvia.</v>
       </c>
-      <c r="M14" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: "función"  
-Fase 2 · Explicación  
-Las &lt;strong&gt;defensas&lt;/strong&gt; se utilizan para proteger el casco del barco y el muelle de posibles daños durante las maniobras de atraque y desatraque. Se colocan provisionalmente en los costados del barco y el muelle para evitar rozamientos o golpes.</v>
-      </c>
-      <c r="N14" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: función
-Fase 2 · Explicación: Las &lt;strong&gt;defensas&lt;/strong&gt; son dispositivos que se colocan en los costados de una embarcación para protegerla de golpes contra el muelle u otras embarcaciones. No están conectadas con alarmas, ya que su propósito principal es evitar daños físicos al actuar como un amortiguador.</v>
-      </c>
-      <c r="O14" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:** La pregunta se clasifica como "localización" porque está preguntando dónde se colocan las defensas en una embarcación.
-**Fase 2 · Explicación:** Las &lt;strong&gt;defensas&lt;/strong&gt; se colocan a lo largo del costado de la embarcación, no solo en la proa, para protegerla contra daños al atracar o al estar junto a otras embarcaciones. Su función principal es absorber impactos y evitar daños en el casco.</v>
-      </c>
-      <c r="P14" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: función
-Fase 2 · Explicación: Las &lt;strong&gt;defensas&lt;/strong&gt; se utilizan para proteger el casco de una embarcación contra daños durante el atraque y las maniobras en el puerto, no para "aislar los portillos del agua de lluvia". Además, se colocan generalmente en los costados de la embarcación y no tienen relación con los portillos o ventanas.</v>
-      </c>
-    </row>
-    <row r="15" xml:space="preserve">
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
+        <v/>
+      </c>
+      <c r="O14" t="str">
+        <v/>
+      </c>
+      <c r="P14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1212,7 +1116,7 @@
         <v>Noray</v>
       </c>
       <c r="E15" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1235,24 +1139,20 @@
       <c r="L15" t="str">
         <v>Viento de Levante</v>
       </c>
-      <c r="M15" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:** definición
-**Fase 2 · Explicación:** Un &lt;strong&gt;noray&lt;/strong&gt; es un elemento de amarre que se ubica en los muelles o puertos para fijar las embarcaciones mediante cabos o cadenas. Aunque un bolardo también se utiliza para atar barcos, el término correcto para este contexto es noray.</v>
-      </c>
-      <c r="N15" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Un &lt;strong&gt;noray&lt;/strong&gt; es un elemento fijo en los puertos, utilizado para amarrar las embarcaciones mediante cabos. No es una vela para mal tiempo; su función es proporcionar un punto de anclaje seguro para asegurar los barcos.</v>
-      </c>
-      <c r="O15" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Un &lt;strong&gt;noray&lt;/strong&gt; es un sólido elemento de amarre, generalmente hecho de metal, ubicado en los muelles para sujetar las amarras de las embarcaciones. No guarda relación con la unión del timón con la embarcación.</v>
-      </c>
-      <c r="P15" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Un &lt;strong&gt;noray&lt;/strong&gt; es un poste fijo en los muelles al que se amarran las embarcaciones mediante cabos. La opción "Viento de Levante" no es correcta; un noray no tiene relación con los vientos, ya que su función es proporcionar un punto de amarre.</v>
-      </c>
-    </row>
-    <row r="16" xml:space="preserve">
+      <c r="M15" t="str">
+        <v/>
+      </c>
+      <c r="N15" t="str">
+        <v/>
+      </c>
+      <c r="O15" t="str">
+        <v/>
+      </c>
+      <c r="P15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1266,7 +1166,7 @@
         <v>Orinque</v>
       </c>
       <c r="E16" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1289,26 +1189,20 @@
       <c r="L16" t="str">
         <v>Aprisionar la cadena del buque y así evitar que se file.</v>
       </c>
-      <c r="M16" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: función
-Fase 2 · Explicación: El &lt;strong&gt;orinque&lt;/strong&gt; es una cuerda que se ata al ancla y que lleva un pequeño flotador en el extremo para señalar la ubicación precisa del ancla fondeada bajo el agua. Esto permite que la tripulación sepa dónde está el ancla y facilita su recuperación.</v>
-      </c>
-      <c r="N16" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: función.
-Fase 2 · Explicación: El &lt;strong&gt;orinque&lt;/strong&gt; es una cuerda o cabo que se utiliza para facilitar el izado o recuperación de una boya, ancla o elemento sumergido. No se emplea para pulir las superficies metálicas del barco.</v>
-      </c>
-      <c r="O16" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: función
-Fase 2 · Explicación: El &lt;strong&gt;orinque&lt;/strong&gt; es una cuerda utilizada para facilitar la recuperación de un ancla. No tiene relación con trincar el aparejo de un buque, que implica asegurar o ajustar las velas y otros elementos del barco.</v>
-      </c>
-      <c r="P16" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación:  
-La pregunta es de tipo "función" porque indaga para qué sirve el "orinque".
-Fase 2 · Explicación:  
-Un &lt;strong&gt;orinque&lt;/strong&gt; es una línea que conecta una boya a un ancla o a otro objeto sumergido para permitir su localización y recuperación. Se utiliza principalmente para señalar la posición de un ancla o para permitir su posterior recuperación desde la superficie.</v>
-      </c>
-    </row>
-    <row r="17" xml:space="preserve">
+      <c r="M16" t="str">
+        <v/>
+      </c>
+      <c r="N16" t="str">
+        <v/>
+      </c>
+      <c r="O16" t="str">
+        <v/>
+      </c>
+      <c r="P16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1322,7 +1216,7 @@
         <v>Línea de fondeo</v>
       </c>
       <c r="E17" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1345,26 +1239,20 @@
       <c r="L17" t="str">
         <v>Mosquetón</v>
       </c>
-      <c r="M17" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: En el contexto náutico, una &lt;strong&gt;Línea de fondeo&lt;/strong&gt; se refiere al conjunto de elementos utilizados para asegurar una embarcación al fondo marino, e incluye la cadena de fondeo, donde cada tramo de 25 metros es conocido como &lt;strong&gt;grillete&lt;/strong&gt;.</v>
-      </c>
-      <c r="N17" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Clasificación:** definición
-**Explicación:** Una &lt;strong&gt;línea de fondeo&lt;/strong&gt; es un conjunto de elementos utilizado para mantener una embarcación fija en el agua, y está compuesta generalmente por un ancla, cadena, cabo y boyas. Cada tramo de cadena de fondeo de 25 metros en la jerga náutica se conoce como "grillete", no "contrete".</v>
-      </c>
-      <c r="O17" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:**  
-La pregunta parece ser una solicitud de definición en el contexto de la náutica.
-**Fase 2 · Explicación:**  
-En el ámbito náutico, un **cáncamo** es un herraje metálico en forma de anillo sujeto a una superficie, utilizado principalmente para fijar y asegurar cabos o cadenas. Sin embargo, en náutica, el término específico para un tramo de 25 metros de cadena de fondeo es "grillete".</v>
-      </c>
-      <c r="P17" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: verdadero_falso
-Fase 2 · Explicación: En términos de náutica, un &lt;strong&gt;mosquetón&lt;/strong&gt; es un tipo de hebilla metálica que se utiliza para unir o asegurar cabos y cables. Sin embargo, no es el término correcto para denominar los tramos de la &lt;strong&gt;línea de fondeo&lt;/strong&gt;; estos se conocen como "grilletes" o "longitudes".</v>
-      </c>
-    </row>
-    <row r="18" xml:space="preserve">
+      <c r="M17" t="str">
+        <v/>
+      </c>
+      <c r="N17" t="str">
+        <v/>
+      </c>
+      <c r="O17" t="str">
+        <v/>
+      </c>
+      <c r="P17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1378,7 +1266,7 @@
         <v>Seno</v>
       </c>
       <c r="E18" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -1401,26 +1289,20 @@
       <c r="L18" t="str">
         <v>Vuelta.</v>
       </c>
-      <c r="M18" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: "definición"
-Fase 2 · Explicación  
-El término &lt;strong&gt;seno&lt;/strong&gt; en náutica no se refiere a la curvatura de un cabo entre los extremos que lo sujetan. En contextos más generales, &lt;strong&gt;seno&lt;/strong&gt; puede referirse a una parte de una curva o a la parte interna de un elemento arqueado, pero no es un término específico para describir la curvatura de un cabo.</v>
-      </c>
-      <c r="N18" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición.
-Fase 2 · Explicación: La curvatura del cabo que hay entre los extremos que lo sujetan se denomina &lt;strong&gt;seno&lt;/strong&gt;. Por otro lado, el término &lt;strong&gt;chicote&lt;/strong&gt; hace referencia al extremo libre de un cabo en náutica.</v>
-      </c>
-      <c r="O18" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: En el contexto de la navegación o náutica, el término &lt;strong&gt;Arco&lt;/strong&gt; no se refiere al seno de la curvatura de un cabo. El &lt;strong&gt;Seno&lt;/strong&gt; es la curvatura que forma un cabo entre sus extremos; debe aclararse que "seno" se utiliza habitualmente en este contexto para describir la flexión natural de un cabo bajo tensión o al ser suspendido.</v>
-      </c>
-      <c r="P18" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: En el contexto náutico, el &lt;strong&gt;seno&lt;/strong&gt; es la parte curvada de un cabo entre sus dos extremos. La opción "vuelta" no se refiere a esta curvatura; en náutica, "vuelta" se utiliza para describir una forma de sujetar un cabo a una bita o cornamusa.</v>
-      </c>
-    </row>
-    <row r="19" xml:space="preserve">
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <v/>
+      </c>
+      <c r="P18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1434,7 +1316,7 @@
         <v>Defensas</v>
       </c>
       <c r="E19" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1457,30 +1339,20 @@
       <c r="L19" t="str">
         <v>Ariete.</v>
       </c>
-      <c r="M19" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:**  
-La pregunta se centra en la función que tiene el objeto mencionado. Por ello, el tipo de pregunta es "función".
-**Fase 2 · Explicación:**  
-Las **defensas** son dispositivos utilizados en embarcaciones para amortiguar y proteger el casco de golpes o roces al atracar o al realizar maniobras cercanas a otras naves o muelles. Actúan como barreras amortiguadoras, garantizando la integridad estructural del barco.</v>
-      </c>
-      <c r="N19" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación**  
-Tipo de pregunta: "función"
-**Fase 2 · Explicación**  
-El concepto &lt;strong&gt;Defensas&lt;/strong&gt; se refiere a un utensilio utilizado para proteger las embarcaciones de roces o golpes al atracar, comúnmente fabricado de materiales como caucho o plástico inflable, que se coloca a lo largo del casco. La opción "Entorchado" no es un término correcto en este contexto, pues el entorchado generalmente se refiere al acto de hacer girar o retorcer algo, como una cuerda.</v>
-      </c>
-      <c r="O19" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación**: La pregunta corresponde al tipo "función", ya que indaga sobre el propósito o uso de un utensilio específico.
-**Fase 2 · Explicación**: Un &lt;strong&gt;sobrante&lt;/strong&gt; no es un término náutico relacionado con la protección de embarcaciones. El término correcto es &lt;strong&gt;defensas&lt;/strong&gt;, que son dispositivos utilizados para proteger las embarcaciones del roce o de golpes al atracar.</v>
-      </c>
-      <c r="P19" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación**  
-Tipo de pregunta: "definición"  
-**Fase 2 · Explicación**  
-El término destacado debería ser **Defensas**, que son dispositivos utilizados para proteger las embarcaciones evitando que sufran daños por roces o golpes cuando están atracando o en contacto con otras embarcaciones. La opción "Ariete" no es correcta en este contexto, ya que un ariete se refiere a un instrumento de impacto o a un carnero hidraúlico, no relacionado con las funciones de defensa en barcos.</v>
-      </c>
-    </row>
-    <row r="20" xml:space="preserve">
+      <c r="M19" t="str">
+        <v/>
+      </c>
+      <c r="N19" t="str">
+        <v/>
+      </c>
+      <c r="O19" t="str">
+        <v/>
+      </c>
+      <c r="P19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1494,7 +1366,7 @@
         <v>Bitas</v>
       </c>
       <c r="E20" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1517,28 +1389,20 @@
       <c r="L20" t="str">
         <v>Pasamanos.</v>
       </c>
-      <c r="M20" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: "función"
-Fase 2 · Explicación  
-Las &lt;strong&gt;bitas&lt;/strong&gt; son piezas metálicas en una embarcación que se utilizan para afirmar o asegurar cabos de amarre, permitiendo que la embarcación quede firmemente sujetada a un muelle o a otra embarcación.</v>
-      </c>
-      <c r="N20" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Las &lt;strong&gt;bitas&lt;/strong&gt; son piezas metálicas instaladas generalmente en las cubiertas de los barcos, diseñadas especialmente para asegurar y amarrar cabos, cuerdas o cables de amarre. Estas sirven de punto de anclaje, permitiendo que las embarcaciones se fijen de manera segura a un muelle o puerto.</v>
-      </c>
-      <c r="O20" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Las &lt;strong&gt;Bitas&lt;/strong&gt; son piezas metálicas ubicadas en embarcaciones que se utilizan para asegurar cabos de amarre. Estas estructuras permiten fijar de manera segura los cabos para mantener el barco en su posición en el muelle.</v>
-      </c>
-      <c r="P20" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: definición
-Fase 2 · Explicación  
-Los &lt;strong&gt;pasamanos&lt;/strong&gt; son elementos de seguridad colocados en las embarcaciones para que las personas puedan sujetarse al moverse por la cubierta. No sirven para afirmar cabos de amarre; ese es el propósito de las &lt;strong&gt;bitas&lt;/strong&gt;.</v>
-      </c>
-    </row>
-    <row r="21" xml:space="preserve">
+      <c r="M20" t="str">
+        <v/>
+      </c>
+      <c r="N20" t="str">
+        <v/>
+      </c>
+      <c r="O20" t="str">
+        <v/>
+      </c>
+      <c r="P20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1552,7 +1416,7 @@
         <v>Unknown</v>
       </c>
       <c r="E21" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1575,28 +1439,20 @@
       <c r="L21" t="str">
         <v>Chocar con algo que flote.</v>
       </c>
-      <c r="M21" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1: Clasificación  
-La pregunta es de tipo "definición", ya que pide qué es algo.
-Fase 2: Explicación  
-&lt;strong&gt;Garrear&lt;/strong&gt; se refiere al acto de que un ancla no se mantenga fija y sea arrastrada por el fondo marino. Esto puede suceder si el viento o las corrientes son demasiado fuertes o si el ancla no está bien agarrada al suelo, afectando la estabilidad de la embarcación.</v>
-      </c>
-      <c r="N21" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: "definición"  
-Fase 2 · Explicación: El término &lt;strong&gt;garrear&lt;/strong&gt; se refiere a la acción de un barco cuando es movido de su posición por la corriente o el viento mientras su ancla está echada, no a "dar vueltas alrededor del ancla". Cuando un barco garrea, significa que el ancla no está bien agarrada al fondo, lo que puede representar un riesgo si no se corrige.</v>
-      </c>
-      <c r="O21" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-La pregunta solicita una definición ya que busca entender qué significa el término "Garrear".
-Fase 2 · Explicación  
-El término &lt;strong&gt;garrear&lt;/strong&gt; en el contexto náutico se refiere a cuando un ancla no se agarra correctamente al fondo y la embarcación se mueve con la corriente o el viento, lo que no implica rozar el casco con el muelle. Rozar el casco con el muelle sería simplemente un error operativo durante las maniobras de atraque.</v>
-      </c>
-      <c r="P21" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: &lt;strong&gt;Garrear&lt;/strong&gt; es un término náutico que se refiere al movimiento no deseado de un barco al arrastrar su ancla por el fondo del agua, en lugar de mantenerse firme en un lugar. No tiene que ver con chocar con algo que flote, sino con la falta de agarre del ancla.</v>
-      </c>
-    </row>
-    <row r="22" xml:space="preserve">
+      <c r="M21" t="str">
+        <v/>
+      </c>
+      <c r="N21" t="str">
+        <v/>
+      </c>
+      <c r="O21" t="str">
+        <v/>
+      </c>
+      <c r="P21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1610,7 +1466,7 @@
         <v>Muertos</v>
       </c>
       <c r="E22" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1633,28 +1489,20 @@
       <c r="L22" t="str">
         <v>Argolla.</v>
       </c>
-      <c r="M22" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: localización
-Fase 2 · Explicación: El concepto de &lt;strong&gt;Muerto&lt;/strong&gt; en el contexto náutico no se refiere a algo que se pueda afirmar en un muelle. Un &lt;strong&gt;muerto&lt;/strong&gt; suele ser un ancla sumergida, utilizada para mantener una embarcación en su lugar, y se encuentra en el fondo del cuerpo de agua, no en el muelle.</v>
-      </c>
-      <c r="N22" t="str" xml:space="preserve">
-        <v xml:space="preserve">### Fase 1 · Clasificación
-Tipo de pregunta: **localización**
-### Fase 2 · Explicación
-Un &lt;strong&gt;muerto&lt;/strong&gt; es un cuerpo sumergido, generalmente una estructura de hormigón, que se utiliza para anclar embarcaciones en su lugar y no se encuentra afirmado en el muelle. En cambio, un &lt;strong&gt;bolardo&lt;/strong&gt; es un poste firme ubicado en un muelle al que se atan las amarras para asegurar la embarcación.</v>
-      </c>
-      <c r="O22" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: localización
-Fase 2 · Explicación: Un &lt;strong&gt;noray&lt;/strong&gt; es un elemento que se encuentra en los muelles y al que se amarran las embarcaciones. Suele estar afirmado en el muelle, a diferencia de los &lt;strong&gt;muertos&lt;/strong&gt;, que son elementos sumergidos y anclados en el fondo del agua.</v>
-      </c>
-      <c r="P22" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:**  
-El tipo de pregunta es "localización", ya que se pregunta por un elemento que no se encuentra afirmado en el muelle.
-**Fase 2 · Explicación:**  
-Una &lt;strong&gt;argolla&lt;/strong&gt; es un dispositivo metálico en forma de anillo que suele utilizarse para sujetar cabos o amarras. No es común que una argolla esté afirmada en un muelle, ya que se utilizan otros sistemas como bolardos o cornamusas para esta función.</v>
-      </c>
-    </row>
-    <row r="23" xml:space="preserve">
+      <c r="M22" t="str">
+        <v/>
+      </c>
+      <c r="N22" t="str">
+        <v/>
+      </c>
+      <c r="O22" t="str">
+        <v/>
+      </c>
+      <c r="P22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1668,7 +1516,7 @@
         <v>Estopor</v>
       </c>
       <c r="E23" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1691,26 +1539,20 @@
       <c r="L23" t="str">
         <v>Lanzada.</v>
       </c>
-      <c r="M23" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: Un &lt;strong&gt;Estopor&lt;/strong&gt; es un mecanismo de hierro que se utiliza en embarcaciones para morder y detener a voluntad la cadena del ancla, asegurando que esta no se desplace de forma no deseada. Se utiliza para controlar y asegurar el ancla cuando está fondeada o durante operaciones de anclaje.</v>
-      </c>
-      <c r="N23" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:** función
-**Fase 2 · Explicación:** El término correcto es &lt;strong&gt;Estopor&lt;/strong&gt;, un mecanismo de hierro en la náutica que sirve para morder y detener a voluntad la cadena de un ancla. No existe un término náutico denominado "Esbotor", por lo que es importante utilizar el nombre adecuado para referirse a este dispositivo.</v>
-      </c>
-      <c r="O23" t="str" xml:space="preserve">
-        <v xml:space="preserve">### Fase 1 · Clasificación
-Tipo de pregunta: **definición**
-### Fase 2 · Explicación
-El término **estupor** no se refiere a un mecanismo de hierro que sirva para morder y detener la cadena en náutica. El mecanismo correcto es el **estopor**, un aparato utilizado en barcos para mantener las cadenas de anclas en su lugar.</v>
-      </c>
-      <c r="P23" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:** función
-**Fase 2 · Explicación:** Un &lt;strong&gt;estopor&lt;/strong&gt; es un mecanismo de hierro utilizado en el ámbito náutico para sujetar y detener a voluntad la cadena del ancla, previniendo que se deslice o pierda tensión cuando no es deseado. Su función es esencial para garantizar la seguridad y control del anclaje en una embarcación.</v>
-      </c>
-    </row>
-    <row r="24" xml:space="preserve">
+      <c r="M23" t="str">
+        <v/>
+      </c>
+      <c r="N23" t="str">
+        <v/>
+      </c>
+      <c r="O23" t="str">
+        <v/>
+      </c>
+      <c r="P23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1724,7 +1566,7 @@
         <v>Garreo</v>
       </c>
       <c r="E24" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -1747,28 +1589,20 @@
       <c r="L24" t="str">
         <v>Chocar con algo que flote.</v>
       </c>
-      <c r="M24" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: "definición"
-Fase 2 · Explicación  
-&lt;strong&gt;Garreo&lt;/strong&gt; consiste en el deslizamiento involuntario del ancla sobre el fondo marino. Esto ocurre cuando el ancla no logra fijarse adecuadamente, provocando que la embarcación no se mantenga en la posición deseada.</v>
-      </c>
-      <c r="N24" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: definición
-Fase 2 · Explicación: &lt;strong&gt;Garreo&lt;/strong&gt; se refiere al movimiento no deseado de un barco cuando su ancla resbala en el fondo marino. Este fenómeno ocurre cuando el ancla no está bien afirmada y el barco se desplaza, a veces dando lugar a "dar vueltas alrededor del ancla", pero principalmente a moverse de su posición original.</v>
-      </c>
-      <c r="O24" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta se enfoca en definir qué es &lt;strong&gt;Garreo&lt;/strong&gt;, por lo tanto es de tipo "definición".
-Fase 2 · Explicación: &lt;strong&gt;Garreo&lt;/strong&gt; en el contexto náutico se refiere a cuando un ancla no agarra adecuadamente y la embarcación se mueve fuera de su posición debido al viento o la corriente. La opción mencionada ("rozar el casco con el muelle") no es correcta, ya que garrear no implica contacto físico con el muelle, sino el movimiento no controlado del barco.</v>
-      </c>
-      <c r="P24" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: *definición*
-Fase 2 · Explicación  
-El término &lt;strong&gt;garrear&lt;/strong&gt; se refiere a la acción de un ancla que pierde su agarre en el fondo marino, provocando que la embarcación se desplace involuntariamente. No está relacionado con chocar contra objetos flotantes.</v>
-      </c>
-    </row>
-    <row r="25" xml:space="preserve">
+      <c r="M24" t="str">
+        <v/>
+      </c>
+      <c r="N24" t="str">
+        <v/>
+      </c>
+      <c r="O24" t="str">
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" t="str">
         <v>amarre-fondeo</v>
       </c>
@@ -1782,7 +1616,7 @@
         <v>Equipo de fondeo</v>
       </c>
       <c r="E25" t="str">
-        <v>M</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1805,25 +1639,17 @@
       <c r="L25" t="str">
         <v>Junto al motor.</v>
       </c>
-      <c r="M25" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación  
-Tipo de pregunta: "localización"
-Fase 2 · Explicación  
-El &lt;strong&gt;equipo de fondeo&lt;/strong&gt; se encuentra habitualmente a proa de la embarcación, ya que esta ubicación facilita el proceso de anclaje en el agua.</v>
-      </c>
-      <c r="N25" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:**  
-El tipo de pregunta según el contexto es "localización", ya que está preguntando dónde se encuentra el **equipo de fondeo**.  
-**Fase 2 · Explicación:**  
-El **equipo de fondeo** generalmente se encuentra en la proa de la embarcación. Sin embargo, en algunas configuraciones, puede estar accesible desde la bañera para manejo conveniente por parte del patrón.</v>
-      </c>
-      <c r="O25" t="str" xml:space="preserve">
-        <v xml:space="preserve">Fase 1 · Clasificación: La pregunta es de tipo "localización", ya que se pregunta por la ubicación del &lt;strong&gt;equipo de fondeo&lt;/strong&gt;.
-Fase 2 · Explicación: El &lt;strong&gt;equipo de fondeo&lt;/strong&gt;, que incluye elementos como el ancla y las cadenas, suele encontrarse en la proa de la embarcación, no en el camarote del Capitán. Su correcta ubicación es esencial para asegurar la estabilidad y seguridad al fondear.</v>
-      </c>
-      <c r="P25" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Fase 1 · Clasificación:** La pregunta es de tipo "localización" porque se pregunta dónde se encuentra el equipo de fondeo.
-**Fase 2 · Explicación:** El &lt;strong&gt;equipo de fondeo&lt;/strong&gt;, que incluye principalmente el ancla y sus accesorios, usualmente se encuentra en la proa de la embarcación y no junto al motor.</v>
+      <c r="M25" t="str">
+        <v/>
+      </c>
+      <c r="N25" t="str">
+        <v/>
+      </c>
+      <c r="O25" t="str">
+        <v/>
+      </c>
+      <c r="P25" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>